<commit_message>
Update Weekly Plan: 8th (2nd)
</commit_message>
<xml_diff>
--- a/07_Report/Weekly Report/Weekly_Plan.xlsx
+++ b/07_Report/Weekly Report/Weekly_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\documents\NMCNPM\ISE_NTMT_01\07_Report\Weekly Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B461CF-501B-47EF-BA52-A82F633C12B5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D4E2F7-80B0-4415-93B5-B2EE3C900104}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8100" activeTab="2" xr2:uid="{F532BE21-CC2C-4AAF-931C-FEA693C31C50}"/>
   </bookViews>
@@ -764,45 +764,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -823,26 +784,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1176,7 +1176,7 @@
       <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="41" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1190,7 +1190,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
+      <c r="A3" s="42"/>
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -1202,33 +1202,33 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="32"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="11"/>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
     </row>
     <row r="6" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="41" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="37"/>
+      <c r="D7" s="48"/>
     </row>
     <row r="8" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="32"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="39"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="50"/>
     </row>
     <row r="10" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="44" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="14" t="s">
@@ -1242,7 +1242,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
+      <c r="A12" s="45"/>
       <c r="B12" s="15">
         <v>1</v>
       </c>
@@ -1254,7 +1254,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="15">
         <v>2</v>
       </c>
@@ -1266,7 +1266,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="15">
         <v>3</v>
       </c>
@@ -1278,7 +1278,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="35"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="11">
         <v>4</v>
       </c>
@@ -1322,7 +1322,7 @@
       <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="44" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -1336,7 +1336,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
+      <c r="A3" s="45"/>
       <c r="B3" s="15">
         <v>1</v>
       </c>
@@ -1348,7 +1348,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="15">
         <v>2</v>
       </c>
@@ -1360,7 +1360,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="15">
         <v>3</v>
       </c>
@@ -1372,7 +1372,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35"/>
+      <c r="A6" s="46"/>
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -1398,30 +1398,30 @@
       <c r="E8" s="16"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="41" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="37"/>
+      <c r="D9" s="48"/>
     </row>
     <row r="10" spans="1:5" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="11">
         <v>1</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="41"/>
+      <c r="D10" s="52"/>
     </row>
     <row r="12" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="44" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1435,7 +1435,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="10">
         <v>1</v>
       </c>
@@ -1447,7 +1447,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
+      <c r="A15" s="45"/>
       <c r="B15" s="10">
         <v>2</v>
       </c>
@@ -1459,7 +1459,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="66" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
+      <c r="A16" s="45"/>
       <c r="B16" s="10">
         <v>3</v>
       </c>
@@ -1471,7 +1471,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="10">
         <v>4</v>
       </c>
@@ -1483,7 +1483,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="66" x14ac:dyDescent="0.25">
-      <c r="A18" s="42"/>
+      <c r="A18" s="53"/>
       <c r="B18" s="10">
         <v>5</v>
       </c>
@@ -1495,7 +1495,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="66" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
+      <c r="A19" s="53"/>
       <c r="B19" s="10">
         <v>6</v>
       </c>
@@ -1507,7 +1507,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
+      <c r="A20" s="53"/>
       <c r="B20" s="10">
         <v>7</v>
       </c>
@@ -1519,7 +1519,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="99" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
+      <c r="A21" s="53"/>
       <c r="B21" s="10">
         <v>8</v>
       </c>
@@ -1531,7 +1531,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="99" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
+      <c r="A22" s="53"/>
       <c r="B22" s="10">
         <v>9</v>
       </c>
@@ -1543,7 +1543,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="99" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
+      <c r="A23" s="53"/>
       <c r="B23" s="10">
         <v>10</v>
       </c>
@@ -1555,7 +1555,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="66.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+      <c r="A24" s="46"/>
       <c r="B24" s="10">
         <v>11</v>
       </c>
@@ -1582,8 +1582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31647020-419D-439C-B043-F5C45F281E94}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1599,34 +1599,34 @@
     </row>
     <row r="5" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="36" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="55">
+      <c r="A7" s="42"/>
+      <c r="B7" s="38">
         <v>1</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="57">
+      <c r="D7" s="40">
         <v>0</v>
       </c>
       <c r="E7" s="16"/>
     </row>
     <row r="8" spans="1:5" ht="33" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="10">
         <v>2</v>
       </c>
@@ -1639,7 +1639,7 @@
       <c r="E8" s="16"/>
     </row>
     <row r="9" spans="1:5" ht="66" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="10">
         <v>3</v>
       </c>
@@ -1651,7 +1651,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="10">
         <v>4</v>
       </c>
@@ -1662,8 +1662,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="66" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+    <row r="11" spans="1:5" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="42"/>
       <c r="B11" s="10">
         <v>5</v>
       </c>
@@ -1674,8 +1674,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="66" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+    <row r="12" spans="1:5" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="42"/>
       <c r="B12" s="10">
         <v>6</v>
       </c>
@@ -1687,7 +1687,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="33" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="10">
         <v>7</v>
       </c>
@@ -1698,8 +1698,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="99" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+    <row r="14" spans="1:5" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="42"/>
       <c r="B14" s="10">
         <v>8</v>
       </c>
@@ -1710,8 +1710,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="99" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+    <row r="15" spans="1:5" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="42"/>
       <c r="B15" s="10">
         <v>9</v>
       </c>
@@ -1723,7 +1723,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="82.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="10">
         <v>10</v>
       </c>
@@ -1735,7 +1735,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="32"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="11">
         <v>11</v>
       </c>
@@ -1743,57 +1743,57 @@
         <v>19</v>
       </c>
       <c r="D17" s="29">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="53" t="s">
+      <c r="C20" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="54"/>
+      <c r="D20" s="55"/>
     </row>
     <row r="21" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="32"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
+      <c r="A21" s="43"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="57"/>
     </row>
     <row r="23" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="48" t="s">
+      <c r="C24" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="49" t="s">
+      <c r="D24" s="36" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
-      <c r="B25" s="44">
+      <c r="A25" s="45"/>
+      <c r="B25" s="31">
         <v>1</v>
       </c>
-      <c r="C25" s="45" t="s">
+      <c r="C25" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="46">
+      <c r="D25" s="33">
         <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
+      <c r="A26" s="45"/>
       <c r="B26" s="15">
         <v>2</v>
       </c>
@@ -1805,7 +1805,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+      <c r="A27" s="45"/>
       <c r="B27" s="15">
         <v>3</v>
       </c>
@@ -1817,7 +1817,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
+      <c r="A28" s="45"/>
       <c r="B28" s="15">
         <v>4</v>
       </c>
@@ -1829,11 +1829,11 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="34"/>
+      <c r="A29" s="45"/>
       <c r="B29" s="15">
         <v>5</v>
       </c>
-      <c r="C29" s="43" t="s">
+      <c r="C29" s="30" t="s">
         <v>28</v>
       </c>
       <c r="D29" s="25">
@@ -1841,11 +1841,11 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="34"/>
+      <c r="A30" s="45"/>
       <c r="B30" s="15">
         <v>6</v>
       </c>
-      <c r="C30" s="43" t="s">
+      <c r="C30" s="30" t="s">
         <v>29</v>
       </c>
       <c r="D30" s="25">
@@ -1853,7 +1853,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="34"/>
+      <c r="A31" s="45"/>
       <c r="B31" s="15">
         <v>7</v>
       </c>
@@ -1863,7 +1863,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
+      <c r="A32" s="46"/>
       <c r="B32" s="11">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Reinit Source; Basic UI: Home Page
</commit_message>
<xml_diff>
--- a/07_Report/Weekly Report/Weekly_Plan.xlsx
+++ b/07_Report/Weekly Report/Weekly_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\documents\NMCNPM\ISE_NTMT_01\07_Report\Weekly Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D4E2F7-80B0-4415-93B5-B2EE3C900104}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE2EA7A-AF82-46BF-84DF-BF5D81B2F995}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8100" activeTab="2" xr2:uid="{F532BE21-CC2C-4AAF-931C-FEA693C31C50}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
   <si>
     <t>STT</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t xml:space="preserve">Xây dựng chức năng restaurant detail </t>
+  </si>
+  <si>
+    <t>Xây dựng chức năng login</t>
   </si>
 </sst>
 </file>
@@ -1582,8 +1585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31647020-419D-439C-B043-F5C45F281E94}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1857,7 +1860,9 @@
       <c r="B31" s="15">
         <v>7</v>
       </c>
-      <c r="C31" s="12"/>
+      <c r="C31" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="D31" s="25">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
WeekPlan 18th, Update HomePage, Restaurant Detail
</commit_message>
<xml_diff>
--- a/07_Report/Weekly Report/Weekly_Plan.xlsx
+++ b/07_Report/Weekly Report/Weekly_Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\documents\NMCNPM\ISE_NTMT_01\07_Report\Weekly Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CEBDA6-80FB-476B-8529-7AEB1888F9DB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A711A2E-3B74-4253-BCC3-CEF9057282F4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8100" firstSheet="8" activeTab="11" xr2:uid="{F532BE21-CC2C-4AAF-931C-FEA693C31C50}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8100" firstSheet="9" activeTab="12" xr2:uid="{F532BE21-CC2C-4AAF-931C-FEA693C31C50}"/>
   </bookViews>
   <sheets>
     <sheet name="08102018-14102018" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="10122018-16122018" sheetId="10" r:id="rId10"/>
     <sheet name="17122018-23122018" sheetId="11" r:id="rId11"/>
     <sheet name="24122018-30122018" sheetId="12" r:id="rId12"/>
+    <sheet name="31122018-06012019" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="43">
   <si>
     <t>STT</t>
   </si>
@@ -172,6 +173,18 @@
   <si>
     <t>Xây dựng chức năng thông tin tài khoản và cập nhật</t>
   </si>
+  <si>
+    <t>Xây dựng chức năng xóa dish trong manage menu</t>
+  </si>
+  <si>
+    <t>Xây dựng trang manage event</t>
+  </si>
+  <si>
+    <t>Chức năng tìm kiếm</t>
+  </si>
+  <si>
+    <t>Xây dựng chức năng add event</t>
+  </si>
 </sst>
 </file>
 
@@ -768,7 +781,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -932,6 +945,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1883,8 +1903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3549458-7C1E-48F4-8907-06D250643687}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2076,6 +2096,229 @@
     <mergeCell ref="A18:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01671C2-6371-4A41-81A5-93AD585048A7}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="39.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+    </row>
+    <row r="5" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="48"/>
+      <c r="B7" s="64">
+        <v>1</v>
+      </c>
+      <c r="C7" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="66">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="48"/>
+      <c r="B8" s="10">
+        <v>2</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="48"/>
+      <c r="B9" s="10">
+        <v>3</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="48"/>
+      <c r="B10" s="10">
+        <v>4</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="27">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="48"/>
+      <c r="B11" s="10">
+        <v>5</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="27">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="49"/>
+      <c r="B12" s="11">
+        <v>6</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="61"/>
+    </row>
+    <row r="16" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="49"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="63"/>
+    </row>
+    <row r="18" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="51"/>
+      <c r="B20" s="15">
+        <v>1</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="59"/>
+      <c r="B21" s="15">
+        <v>2</v>
+      </c>
+      <c r="C21" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="43">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="59"/>
+      <c r="B22" s="15">
+        <v>3</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="59"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="43">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="59"/>
+      <c r="B24" s="15">
+        <v>4</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="43">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="52"/>
+      <c r="B25" s="44">
+        <v>5</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="26">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A19:A25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>